<commit_message>
fixed issue with deciles
</commit_message>
<xml_diff>
--- a/_site/xls/Income three-year average.xlsx
+++ b/_site/xls/Income three-year average.xlsx
@@ -6,26 +6,26 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Contents" sheetId="219" state="visible" r:id="rId14"/>
-    <sheet name="Median income BHC" sheetId="206" state="visible" r:id="rId1"/>
-    <sheet name="Median income AHC" sheetId="207" state="visible" r:id="rId2"/>
-    <sheet name="Decile points BHC" sheetId="208" state="visible" r:id="rId3"/>
-    <sheet name="Decile points AHC" sheetId="209" state="visible" r:id="rId4"/>
-    <sheet name="Decile shares BHC" sheetId="210" state="visible" r:id="rId5"/>
-    <sheet name="Decile shares AHC" sheetId="211" state="visible" r:id="rId6"/>
-    <sheet name="Palma BHC" sheetId="212" state="visible" r:id="rId7"/>
-    <sheet name="Palma AHC" sheetId="213" state="visible" r:id="rId8"/>
-    <sheet name="Gini BHC" sheetId="214" state="visible" r:id="rId9"/>
-    <sheet name="Gini AHC" sheetId="215" state="visible" r:id="rId10"/>
-    <sheet name="Poverty thresholds BHC" sheetId="216" state="visible" r:id="rId11"/>
-    <sheet name="Poverty thresholds AHC" sheetId="217" state="visible" r:id="rId12"/>
-    <sheet name="Income sources" sheetId="218" state="visible" r:id="rId13"/>
+    <sheet name="Contents" sheetId="233" state="visible" r:id="rId14"/>
+    <sheet name="Median income BHC" sheetId="220" state="visible" r:id="rId1"/>
+    <sheet name="Median income AHC" sheetId="221" state="visible" r:id="rId2"/>
+    <sheet name="Decile points BHC" sheetId="222" state="visible" r:id="rId3"/>
+    <sheet name="Decile points AHC" sheetId="223" state="visible" r:id="rId4"/>
+    <sheet name="Decile shares BHC" sheetId="224" state="visible" r:id="rId5"/>
+    <sheet name="Decile shares AHC" sheetId="225" state="visible" r:id="rId6"/>
+    <sheet name="Palma BHC" sheetId="226" state="visible" r:id="rId7"/>
+    <sheet name="Palma AHC" sheetId="227" state="visible" r:id="rId8"/>
+    <sheet name="Gini BHC" sheetId="228" state="visible" r:id="rId9"/>
+    <sheet name="Gini AHC" sheetId="229" state="visible" r:id="rId10"/>
+    <sheet name="Poverty thresholds BHC" sheetId="230" state="visible" r:id="rId11"/>
+    <sheet name="Poverty thresholds AHC" sheetId="231" state="visible" r:id="rId12"/>
+    <sheet name="Income sources" sheetId="232" state="visible" r:id="rId13"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="1211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="1237">
   <si>
     <t xml:space="preserve">Median income before housing costs by age group</t>
   </si>
@@ -3660,6 +3660,84 @@
   </si>
   <si>
     <t xml:space="preserve">social-justice-analysis@gov.scot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median weekly equivalised household income in £ (in 2018/19 prices), Scotland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1996/97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1997/98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1998/99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1999/00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000/01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001/02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002/03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003/04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004/05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2005/06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2006/07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2007/08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008/09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013/14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median weekly equivalised household income decile points in £ (in 2018/19 prices), Scotland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual household income shares in £ million (in 2018/19 prices), Scotland</t>
   </si>
 </sst>
 </file>
@@ -4127,7 +4205,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="6">
@@ -4149,7 +4227,7 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>
@@ -4166,7 +4244,7 @@
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
@@ -4183,7 +4261,7 @@
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>18</v>
@@ -4200,7 +4278,7 @@
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>23</v>
@@ -4217,7 +4295,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>28</v>
@@ -4234,7 +4312,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>33</v>
@@ -4251,7 +4329,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>38</v>
@@ -4268,7 +4346,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>43</v>
@@ -4285,7 +4363,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>48</v>
@@ -4302,7 +4380,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>52</v>
@@ -4319,7 +4397,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>56</v>
@@ -4336,7 +4414,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>61</v>
@@ -4353,7 +4431,7 @@
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>66</v>
@@ -4370,7 +4448,7 @@
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>45</v>
@@ -4387,7 +4465,7 @@
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>74</v>
@@ -4404,7 +4482,7 @@
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>78</v>
@@ -4421,7 +4499,7 @@
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>82</v>
@@ -4438,7 +4516,7 @@
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>66</v>
@@ -4455,7 +4533,7 @@
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>78</v>
@@ -4472,7 +4550,7 @@
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>45</v>
@@ -4489,7 +4567,7 @@
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>95</v>
@@ -4506,7 +4584,7 @@
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>99</v>
@@ -4523,7 +4601,7 @@
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>103</v>
@@ -4585,7 +4663,7 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>909</v>
@@ -4593,7 +4671,7 @@
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>912</v>
@@ -4601,7 +4679,7 @@
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>912</v>
@@ -4609,7 +4687,7 @@
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>913</v>
@@ -4617,7 +4695,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>914</v>
@@ -4625,7 +4703,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>913</v>
@@ -4633,7 +4711,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>913</v>
@@ -4641,7 +4719,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>912</v>
@@ -4649,7 +4727,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>912</v>
@@ -4657,7 +4735,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>912</v>
@@ -4665,7 +4743,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>912</v>
@@ -4673,7 +4751,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>913</v>
@@ -4681,7 +4759,7 @@
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>914</v>
@@ -4689,7 +4767,7 @@
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>915</v>
@@ -4697,7 +4775,7 @@
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>914</v>
@@ -4705,7 +4783,7 @@
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>913</v>
@@ -4713,7 +4791,7 @@
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>912</v>
@@ -4721,7 +4799,7 @@
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>912</v>
@@ -4729,7 +4807,7 @@
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>912</v>
@@ -4737,7 +4815,7 @@
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>913</v>
@@ -4745,7 +4823,7 @@
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>914</v>
@@ -4753,7 +4831,7 @@
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>914</v>
@@ -4761,7 +4839,7 @@
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>914</v>
@@ -4988,7 +5066,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>1109</v>
+        <v>953</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>954</v>
@@ -5017,7 +5095,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>1110</v>
+        <v>959</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>960</v>
@@ -5046,7 +5124,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>1111</v>
+        <v>965</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>184</v>
@@ -5075,7 +5153,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>1112</v>
+        <v>970</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>21</v>
@@ -5104,7 +5182,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>1113</v>
+        <v>975</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>36</v>
@@ -5133,7 +5211,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>1114</v>
+        <v>976</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>156</v>
@@ -5162,7 +5240,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>1115</v>
+        <v>981</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>30</v>
@@ -5191,7 +5269,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>1116</v>
+        <v>988</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>989</v>
@@ -5219,65 +5297,36 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="5" t="s">
-        <v>1117</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>997</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>998</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="6" t="s">
         <v>999</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="6" t="s">
         <v>1000</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="6" t="s">
         <v>1001</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="6" t="s">
         <v>1002</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="6" t="s">
         <v>1003</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="6" t="s">
-        <v>1118</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>1164</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>1141</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>1166</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>1167</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>1168</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>1169</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>111</v>
       </c>
     </row>
@@ -5504,7 +5553,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>1109</v>
+        <v>953</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>1027</v>
@@ -5533,7 +5582,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>1110</v>
+        <v>959</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>1032</v>
@@ -5562,7 +5611,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>1111</v>
+        <v>965</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>1037</v>
@@ -5591,7 +5640,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>1112</v>
+        <v>970</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>234</v>
@@ -5620,7 +5669,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>1113</v>
+        <v>975</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>122</v>
@@ -5649,7 +5698,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>1114</v>
+        <v>976</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>944</v>
@@ -5678,7 +5727,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>1115</v>
+        <v>981</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>1051</v>
@@ -5707,7 +5756,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>1116</v>
+        <v>988</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>135</v>
@@ -5735,65 +5784,36 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="5" t="s">
-        <v>1117</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>1063</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="6" t="s">
         <v>1064</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="6" t="s">
         <v>1065</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="6" t="s">
         <v>1066</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="6" t="s">
         <v>1067</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="6" t="s">
         <v>1068</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="6" t="s">
-        <v>1118</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>1172</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>1163</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>1173</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>1174</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>1175</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>1176</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>111</v>
       </c>
     </row>
@@ -6264,7 +6284,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="6">
@@ -6286,7 +6306,7 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>113</v>
@@ -6303,7 +6323,7 @@
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>9</v>
@@ -6320,7 +6340,7 @@
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>119</v>
@@ -6337,7 +6357,7 @@
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>123</v>
@@ -6354,7 +6374,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>127</v>
@@ -6371,7 +6391,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -6388,7 +6408,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>133</v>
@@ -6405,7 +6425,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>137</v>
@@ -6422,7 +6442,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>140</v>
@@ -6439,7 +6459,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>144</v>
@@ -6456,7 +6476,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>49</v>
@@ -6473,7 +6493,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>149</v>
@@ -6490,7 +6510,7 @@
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>85</v>
@@ -6507,7 +6527,7 @@
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>155</v>
@@ -6524,7 +6544,7 @@
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>158</v>
@@ -6541,7 +6561,7 @@
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>62</v>
@@ -6558,7 +6578,7 @@
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>57</v>
@@ -6575,7 +6595,7 @@
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>87</v>
@@ -6592,7 +6612,7 @@
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>62</v>
@@ -6609,7 +6629,7 @@
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>30</v>
@@ -6626,7 +6646,7 @@
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>161</v>
@@ -6643,7 +6663,7 @@
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>96</v>
@@ -6660,7 +6680,7 @@
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>105</v>
@@ -6703,7 +6723,6 @@
     <col min="9" max="9" width="3.71" hidden="0" customWidth="1"/>
     <col min="10" max="10" width="3.71" hidden="0" customWidth="1"/>
     <col min="11" max="11" width="3.71" hidden="0" customWidth="1"/>
-    <col min="12" max="12" width="6.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6718,7 +6737,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>170</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
@@ -6752,7 +6771,6 @@
       <c r="K5" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="L5" s="7"/>
     </row>
     <row r="6">
       <c r="B6" s="4" t="s">
@@ -6785,13 +6803,10 @@
       <c r="K6" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>1118</v>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>182</v>
@@ -6820,13 +6835,10 @@
       <c r="K7" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>1119</v>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>190</v>
@@ -6855,13 +6867,10 @@
       <c r="K8" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>1120</v>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>196</v>
@@ -6890,13 +6899,10 @@
       <c r="K9" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>1121</v>
-      </c>
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>202</v>
@@ -6925,13 +6931,10 @@
       <c r="K10" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>1122</v>
-      </c>
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>207</v>
@@ -6960,13 +6963,10 @@
       <c r="K11" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>1123</v>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>213</v>
@@ -6995,13 +6995,10 @@
       <c r="K12" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>1124</v>
-      </c>
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>183</v>
@@ -7030,13 +7027,10 @@
       <c r="K13" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>1125</v>
-      </c>
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>227</v>
@@ -7065,13 +7059,10 @@
       <c r="K14" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>1126</v>
-      </c>
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>234</v>
@@ -7100,13 +7091,10 @@
       <c r="K15" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>1127</v>
-      </c>
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>238</v>
@@ -7135,13 +7123,10 @@
       <c r="K16" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>1128</v>
-      </c>
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>246</v>
@@ -7170,13 +7155,10 @@
       <c r="K17" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>1129</v>
-      </c>
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>252</v>
@@ -7205,13 +7187,10 @@
       <c r="K18" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>1130</v>
-      </c>
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>258</v>
@@ -7240,13 +7219,10 @@
       <c r="K19" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>1131</v>
-      </c>
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>264</v>
@@ -7275,13 +7251,10 @@
       <c r="K20" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>1132</v>
-      </c>
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>114</v>
@@ -7310,13 +7283,10 @@
       <c r="K21" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>1133</v>
-      </c>
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>274</v>
@@ -7345,13 +7315,10 @@
       <c r="K22" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>1134</v>
-      </c>
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>279</v>
@@ -7380,13 +7347,10 @@
       <c r="K23" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>1135</v>
-      </c>
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>279</v>
@@ -7415,13 +7379,10 @@
       <c r="K24" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>1136</v>
-      </c>
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>114</v>
@@ -7450,13 +7411,10 @@
       <c r="K25" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>1137</v>
-      </c>
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>293</v>
@@ -7485,13 +7443,10 @@
       <c r="K26" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>1138</v>
-      </c>
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>298</v>
@@ -7520,13 +7475,10 @@
       <c r="K27" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>1139</v>
-      </c>
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>114</v>
@@ -7555,13 +7507,10 @@
       <c r="K28" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>1140</v>
-      </c>
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>308</v>
@@ -7589,9 +7538,6 @@
       </c>
       <c r="K29" s="6" t="s">
         <v>311</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="30">
@@ -7626,7 +7572,6 @@
     <col min="9" max="9" width="3.71" hidden="0" customWidth="1"/>
     <col min="10" max="10" width="3.71" hidden="0" customWidth="1"/>
     <col min="11" max="11" width="3.71" hidden="0" customWidth="1"/>
-    <col min="12" max="12" width="6.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7641,7 +7586,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>170</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
@@ -7675,7 +7620,6 @@
       <c r="K5" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="L5" s="7"/>
     </row>
     <row r="6">
       <c r="B6" s="4" t="s">
@@ -7708,13 +7652,10 @@
       <c r="K6" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>1118</v>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>322</v>
@@ -7743,13 +7684,10 @@
       <c r="K7" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>1142</v>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>327</v>
@@ -7778,13 +7716,10 @@
       <c r="K8" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>1143</v>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>334</v>
@@ -7813,13 +7748,10 @@
       <c r="K9" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>1144</v>
-      </c>
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>337</v>
@@ -7848,13 +7780,10 @@
       <c r="K10" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>1145</v>
-      </c>
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>341</v>
@@ -7883,13 +7812,10 @@
       <c r="K11" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>1146</v>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>348</v>
@@ -7918,13 +7844,10 @@
       <c r="K12" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>1147</v>
-      </c>
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>323</v>
@@ -7953,13 +7876,10 @@
       <c r="K13" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>1148</v>
-      </c>
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>352</v>
@@ -7988,13 +7908,10 @@
       <c r="K14" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>1149</v>
-      </c>
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>355</v>
@@ -8023,13 +7940,10 @@
       <c r="K15" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>1150</v>
-      </c>
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>190</v>
@@ -8058,13 +7972,10 @@
       <c r="K16" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>592</v>
-      </c>
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>362</v>
@@ -8093,13 +8004,10 @@
       <c r="K17" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>1151</v>
-      </c>
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>366</v>
@@ -8128,13 +8036,10 @@
       <c r="K18" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>1152</v>
-      </c>
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>362</v>
@@ -8163,13 +8068,10 @@
       <c r="K19" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>1153</v>
-      </c>
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>338</v>
@@ -8198,13 +8100,10 @@
       <c r="K20" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>1154</v>
-      </c>
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>378</v>
@@ -8233,13 +8132,10 @@
       <c r="K21" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>1155</v>
-      </c>
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>384</v>
@@ -8268,13 +8164,10 @@
       <c r="K22" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>1156</v>
-      </c>
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>196</v>
@@ -8303,13 +8196,10 @@
       <c r="K23" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>1157</v>
-      </c>
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>190</v>
@@ -8338,13 +8228,10 @@
       <c r="K24" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>1158</v>
-      </c>
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>190</v>
@@ -8373,13 +8260,10 @@
       <c r="K25" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>1159</v>
-      </c>
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>378</v>
@@ -8408,13 +8292,10 @@
       <c r="K26" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>1160</v>
-      </c>
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>396</v>
@@ -8443,13 +8324,10 @@
       <c r="K27" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>1161</v>
-      </c>
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>190</v>
@@ -8478,13 +8356,10 @@
       <c r="K28" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>1162</v>
-      </c>
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>378</v>
@@ -8512,9 +8387,6 @@
       </c>
       <c r="K29" s="6" t="s">
         <v>405</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="30">
@@ -8564,7 +8436,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>407</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
@@ -8639,7 +8511,7 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>418</v>
@@ -8674,7 +8546,7 @@
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>428</v>
@@ -8709,7 +8581,7 @@
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>438</v>
@@ -8744,7 +8616,7 @@
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>448</v>
@@ -8779,7 +8651,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>458</v>
@@ -8814,7 +8686,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>468</v>
@@ -8849,7 +8721,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>478</v>
@@ -8884,7 +8756,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>488</v>
@@ -8919,7 +8791,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>498</v>
@@ -8954,7 +8826,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>508</v>
@@ -8989,7 +8861,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>518</v>
@@ -9024,7 +8896,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>528</v>
@@ -9059,7 +8931,7 @@
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>538</v>
@@ -9094,7 +8966,7 @@
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>548</v>
@@ -9129,7 +9001,7 @@
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>558</v>
@@ -9164,7 +9036,7 @@
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>568</v>
@@ -9199,7 +9071,7 @@
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>578</v>
@@ -9234,7 +9106,7 @@
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>588</v>
@@ -9269,7 +9141,7 @@
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>598</v>
@@ -9304,7 +9176,7 @@
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>608</v>
@@ -9339,7 +9211,7 @@
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>618</v>
@@ -9374,7 +9246,7 @@
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>628</v>
@@ -9409,7 +9281,7 @@
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>638</v>
@@ -9489,7 +9361,7 @@
     </row>
     <row r="3">
       <c r="B3" s="2" t="s">
-        <v>407</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
@@ -9564,7 +9436,7 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>650</v>
@@ -9599,7 +9471,7 @@
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>659</v>
@@ -9634,7 +9506,7 @@
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>669</v>
@@ -9669,7 +9541,7 @@
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>679</v>
@@ -9704,7 +9576,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>688</v>
@@ -9739,7 +9611,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>698</v>
@@ -9774,7 +9646,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>708</v>
@@ -9809,7 +9681,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>717</v>
@@ -9844,7 +9716,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>727</v>
@@ -9879,7 +9751,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>737</v>
@@ -9914,7 +9786,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>746</v>
@@ -9949,7 +9821,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>756</v>
@@ -9984,7 +9856,7 @@
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>765</v>
@@ -10019,7 +9891,7 @@
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>775</v>
@@ -10054,7 +9926,7 @@
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>784</v>
@@ -10089,7 +9961,7 @@
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>793</v>
@@ -10124,7 +9996,7 @@
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>803</v>
@@ -10159,7 +10031,7 @@
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>812</v>
@@ -10194,7 +10066,7 @@
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>821</v>
@@ -10229,7 +10101,7 @@
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>831</v>
@@ -10264,7 +10136,7 @@
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>841</v>
@@ -10299,7 +10171,7 @@
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>851</v>
@@ -10334,7 +10206,7 @@
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>861</v>
@@ -10418,7 +10290,7 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>874</v>
@@ -10426,7 +10298,7 @@
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>875</v>
@@ -10434,7 +10306,7 @@
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>876</v>
@@ -10442,7 +10314,7 @@
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>877</v>
@@ -10450,7 +10322,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>878</v>
@@ -10458,7 +10330,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>879</v>
@@ -10466,7 +10338,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>877</v>
@@ -10474,7 +10346,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>876</v>
@@ -10482,7 +10354,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>880</v>
@@ -10490,7 +10362,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>880</v>
@@ -10498,7 +10370,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>876</v>
@@ -10506,7 +10378,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>881</v>
@@ -10514,7 +10386,7 @@
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>882</v>
@@ -10522,7 +10394,7 @@
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>883</v>
@@ -10530,7 +10402,7 @@
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>884</v>
@@ -10538,7 +10410,7 @@
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>877</v>
@@ -10546,7 +10418,7 @@
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>876</v>
@@ -10554,7 +10426,7 @@
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>875</v>
@@ -10562,7 +10434,7 @@
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>885</v>
@@ -10570,7 +10442,7 @@
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>877</v>
@@ -10578,7 +10450,7 @@
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>886</v>
@@ -10586,7 +10458,7 @@
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>878</v>
@@ -10594,7 +10466,7 @@
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>887</v>
@@ -10647,7 +10519,7 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>882</v>
@@ -10655,7 +10527,7 @@
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>890</v>
@@ -10663,7 +10535,7 @@
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>891</v>
@@ -10671,7 +10543,7 @@
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>892</v>
@@ -10679,7 +10551,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>893</v>
@@ -10687,7 +10559,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>894</v>
@@ -10695,7 +10567,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>892</v>
@@ -10703,7 +10575,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>883</v>
@@ -10711,7 +10583,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>890</v>
@@ -10719,7 +10591,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>890</v>
@@ -10727,7 +10599,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>895</v>
@@ -10735,7 +10607,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>896</v>
@@ -10743,7 +10615,7 @@
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>897</v>
@@ -10751,7 +10623,7 @@
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>898</v>
@@ -10759,7 +10631,7 @@
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>899</v>
@@ -10767,7 +10639,7 @@
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>896</v>
@@ -10775,7 +10647,7 @@
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>900</v>
@@ -10783,7 +10655,7 @@
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>901</v>
@@ -10791,7 +10663,7 @@
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>902</v>
@@ -10799,7 +10671,7 @@
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>903</v>
@@ -10807,7 +10679,7 @@
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>893</v>
@@ -10815,7 +10687,7 @@
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>897</v>
@@ -10823,7 +10695,7 @@
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>894</v>
@@ -10876,7 +10748,7 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>1212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>907</v>
@@ -10884,7 +10756,7 @@
     </row>
     <row r="8">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>1213</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>907</v>
@@ -10892,7 +10764,7 @@
     </row>
     <row r="9">
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>1214</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>907</v>
@@ -10900,7 +10772,7 @@
     </row>
     <row r="10">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>1215</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>908</v>
@@ -10908,7 +10780,7 @@
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>1216</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>909</v>
@@ -10916,7 +10788,7 @@
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>1217</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>909</v>
@@ -10924,7 +10796,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>1218</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>908</v>
@@ -10932,7 +10804,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>1219</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>907</v>
@@ -10940,7 +10812,7 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>1220</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>907</v>
@@ -10948,7 +10820,7 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>1221</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>907</v>
@@ -10956,7 +10828,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>1222</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>907</v>
@@ -10964,7 +10836,7 @@
     </row>
     <row r="18">
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>1223</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>908</v>
@@ -10972,7 +10844,7 @@
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>909</v>
@@ -10980,7 +10852,7 @@
     </row>
     <row r="20">
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>1225</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>909</v>
@@ -10988,7 +10860,7 @@
     </row>
     <row r="21">
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>1226</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>909</v>
@@ -10996,7 +10868,7 @@
     </row>
     <row r="22">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>1227</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>908</v>
@@ -11004,7 +10876,7 @@
     </row>
     <row r="23">
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>1228</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>907</v>
@@ -11012,7 +10884,7 @@
     </row>
     <row r="24">
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>1229</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>907</v>
@@ -11020,7 +10892,7 @@
     </row>
     <row r="25">
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>1230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>907</v>
@@ -11028,7 +10900,7 @@
     </row>
     <row r="26">
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>1231</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>908</v>
@@ -11036,7 +10908,7 @@
     </row>
     <row r="27">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>1232</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>908</v>
@@ -11044,7 +10916,7 @@
     </row>
     <row r="28">
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>1233</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>909</v>
@@ -11052,7 +10924,7 @@
     </row>
     <row r="29">
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>1234</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>908</v>

</xml_diff>